<commit_message>
Cap nhat lai don vi tien
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8554A0E-F48B-4479-A46C-5CF577182E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1104" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
+    <sheet name="Category" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>masp</t>
   </si>
@@ -70,12 +72,99 @@
   </si>
   <si>
     <t>SP69</t>
+  </si>
+  <si>
+    <t>tenloai</t>
+  </si>
+  <si>
+    <t>ML01</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>ML02</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>MSI</t>
+  </si>
+  <si>
+    <t>ML04</t>
+  </si>
+  <si>
+    <t>Realme</t>
+  </si>
+  <si>
+    <t>ML05</t>
+  </si>
+  <si>
+    <t>ML06</t>
+  </si>
+  <si>
+    <t>Vivo</t>
+  </si>
+  <si>
+    <t>ML07</t>
+  </si>
+  <si>
+    <t>Redmi</t>
+  </si>
+  <si>
+    <t>ML08</t>
+  </si>
+  <si>
+    <t>Xiaomi</t>
+  </si>
+  <si>
+    <t>ML09</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>ML10</t>
+  </si>
+  <si>
+    <t>Asus</t>
+  </si>
+  <si>
+    <t>ML11</t>
+  </si>
+  <si>
+    <t>Huewei</t>
+  </si>
+  <si>
+    <t>ML12</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
+  </si>
+  <si>
+    <t>ML13</t>
+  </si>
+  <si>
+    <t>Vsmart</t>
+  </si>
+  <si>
+    <t>ML14</t>
+  </si>
+  <si>
+    <t>VNPT</t>
+  </si>
+  <si>
+    <t>ML15</t>
+  </si>
+  <si>
+    <t>LG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -386,21 +475,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -429,7 +518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -458,7 +547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -485,6 +574,149 @@
       </c>
       <c r="J4">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7684A90A-FECD-44D8-B103-B710AA849F63}">
+  <dimension ref="B2:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>